<commit_message>
Updated supplemental data files
</commit_message>
<xml_diff>
--- a/Supplementary Data Files/Supplementary File 3.xlsx
+++ b/Supplementary Data Files/Supplementary File 3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/jdprest_emory_edu/Documents/Research/Manuscripts and Projects/Active Projects/Thyroid Exposomics Paper/MANUSCRIPT SUBMISSIONS/Thyroid Lancet/Manuscript Submission Materials/Supplementary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1127" documentId="8_{B4A3A8FD-2D75-4F4E-8AE7-7CB7BA630849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FCE6C44-0F9C-4B49-B971-120BCEB3FA12}"/>
+  <xr:revisionPtr revIDLastSave="1131" documentId="8_{B4A3A8FD-2D75-4F4E-8AE7-7CB7BA630849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1156533-18A9-C246-8A58-06313D60C753}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{3C529916-AEB2-5A4C-9AEE-70179AF9DBE7}"/>
+    <workbookView xWindow="-33680" yWindow="23100" windowWidth="28800" windowHeight="18900" xr2:uid="{3C529916-AEB2-5A4C-9AEE-70179AF9DBE7}"/>
   </bookViews>
   <sheets>
     <sheet name="feature_metadata" sheetId="30" r:id="rId1"/>
@@ -10480,9 +10480,6 @@
     <t>benzo[a]pyrene</t>
   </si>
   <si>
-    <t>Benz[a]pyrene</t>
-  </si>
-  <si>
     <t>T3D0152</t>
   </si>
   <si>
@@ -11741,6 +11738,9 @@
   </si>
   <si>
     <t>Octyl-dimethyl-p-aminobenzoic acid</t>
+  </si>
+  <si>
+    <t>Benzo[a]pyrene</t>
   </si>
 </sst>
 </file>
@@ -12257,8 +12257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CEBC29-3567-B44B-81AE-C9A53B403E66}">
   <dimension ref="A1:AD444"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A237" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C254" sqref="C254"/>
+    <sheetView tabSelected="1" topLeftCell="A177" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C195" sqref="C195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12291,94 +12291,94 @@
   <sheetData>
     <row r="1" spans="1:30" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>3685</v>
+        <v>3684</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3684</v>
+        <v>3683</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3683</v>
+        <v>3682</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3682</v>
+        <v>3681</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3681</v>
+        <v>3680</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3680</v>
+        <v>3679</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3679</v>
+        <v>3678</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>3678</v>
+        <v>3677</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>3677</v>
+        <v>3676</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>3676</v>
+        <v>3675</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>3675</v>
+        <v>3674</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>3674</v>
+        <v>3673</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>3673</v>
+        <v>3672</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>3672</v>
+        <v>3671</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>3671</v>
+        <v>3670</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>3670</v>
+        <v>3669</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>3669</v>
+        <v>3668</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>3668</v>
+        <v>3667</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>3667</v>
+        <v>3666</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>3666</v>
+        <v>3665</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>3665</v>
+        <v>3664</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>3664</v>
+        <v>3663</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>3663</v>
+        <v>3662</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>3662</v>
+        <v>3661</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>3660</v>
+        <v>3659</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>3659</v>
+        <v>3658</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>3658</v>
+        <v>3657</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>3657</v>
+        <v>3656</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>3656</v>
+        <v>3655</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
@@ -12389,7 +12389,7 @@
         <v>105</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3886</v>
+        <v>3885</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3075</v>
@@ -12473,7 +12473,7 @@
         <v>105</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>3887</v>
+        <v>3886</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>695</v>
@@ -12553,7 +12553,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>3888</v>
+        <v>3887</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>849</v>
@@ -12635,7 +12635,7 @@
         <v>105</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>3889</v>
+        <v>3888</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>2684</v>
@@ -12715,7 +12715,7 @@
         <v>105</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>3890</v>
+        <v>3889</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>2788</v>
@@ -12795,7 +12795,7 @@
         <v>105</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>3891</v>
+        <v>3890</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>3461</v>
@@ -12877,7 +12877,7 @@
         <v>105</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>3892</v>
+        <v>3891</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>2769</v>
@@ -12959,7 +12959,7 @@
         <v>105</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>3787</v>
+        <v>3786</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>1909</v>
@@ -16867,34 +16867,34 @@
         <v>1</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>3645</v>
+        <v>3644</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>3644</v>
+        <v>3643</v>
       </c>
       <c r="G58" s="2">
         <v>9171</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>3643</v>
+        <v>3642</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>3642</v>
+        <v>3641</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>3641</v>
+        <v>3640</v>
       </c>
       <c r="K58" s="2">
         <v>228.09389999999999</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>3614</v>
+        <v>3613</v>
       </c>
       <c r="M58" s="2">
         <v>0.18333333299999999</v>
@@ -16903,7 +16903,7 @@
         <v>97</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>3640</v>
+        <v>3639</v>
       </c>
       <c r="P58" s="2" t="s">
         <v>14</v>
@@ -16932,10 +16932,10 @@
         <v>1988</v>
       </c>
       <c r="Z58" s="2" t="s">
-        <v>3639</v>
+        <v>3638</v>
       </c>
       <c r="AA58" s="2" t="s">
-        <v>3639</v>
+        <v>3638</v>
       </c>
       <c r="AB58" s="2"/>
       <c r="AC58" s="2"/>
@@ -17417,7 +17417,7 @@
         <v>105</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>3811</v>
+        <v>3810</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>1186</v>
@@ -17493,13 +17493,13 @@
         <v>1</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>3550</v>
+        <v>3549</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>3550</v>
+        <v>3549</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>3549</v>
+        <v>3548</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>83</v>
@@ -17508,19 +17508,19 @@
         <v>16653</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>3548</v>
+        <v>3547</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>3547</v>
+        <v>3546</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>3546</v>
+        <v>3545</v>
       </c>
       <c r="K66" s="2">
         <v>187.10310000000001</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>3545</v>
+        <v>3544</v>
       </c>
       <c r="M66" s="2">
         <v>0</v>
@@ -17529,7 +17529,7 @@
         <v>97</v>
       </c>
       <c r="O66" s="2" t="s">
-        <v>3544</v>
+        <v>3543</v>
       </c>
       <c r="P66" s="2"/>
       <c r="Q66" s="2" t="s">
@@ -17555,11 +17555,11 @@
         <v>218</v>
       </c>
       <c r="Y66" s="2" t="s">
-        <v>3543</v>
+        <v>3542</v>
       </c>
       <c r="Z66" s="2"/>
       <c r="AA66" s="2" t="s">
-        <v>3543</v>
+        <v>3542</v>
       </c>
       <c r="AB66" s="2"/>
       <c r="AC66" s="2"/>
@@ -18835,7 +18835,7 @@
         <v>105</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>3783</v>
+        <v>3782</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>2012</v>
@@ -18915,7 +18915,7 @@
         <v>105</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>3784</v>
+        <v>3783</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>2796</v>
@@ -19555,10 +19555,10 @@
         <v>105</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>3859</v>
+        <v>3858</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>3859</v>
+        <v>3858</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>779</v>
@@ -19637,7 +19637,7 @@
         <v>105</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>3862</v>
+        <v>3861</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>773</v>
@@ -20273,7 +20273,7 @@
         <v>105</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>3771</v>
+        <v>3770</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>2310</v>
@@ -20507,13 +20507,13 @@
         <v>1</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>3593</v>
+        <v>3592</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>3593</v>
+        <v>3592</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>3592</v>
+        <v>3591</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>23</v>
@@ -20522,19 +20522,19 @@
         <v>8418</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>3591</v>
+        <v>3590</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>3590</v>
+        <v>3589</v>
       </c>
       <c r="J104" s="2" t="s">
-        <v>3589</v>
+        <v>3588</v>
       </c>
       <c r="K104" s="2">
         <v>178.07830000000001</v>
       </c>
       <c r="L104" s="2" t="s">
-        <v>3588</v>
+        <v>3587</v>
       </c>
       <c r="M104" s="2">
         <v>0.61666666699999995</v>
@@ -20543,7 +20543,7 @@
         <v>97</v>
       </c>
       <c r="O104" s="2" t="s">
-        <v>3587</v>
+        <v>3586</v>
       </c>
       <c r="P104" s="2" t="s">
         <v>14</v>
@@ -20743,7 +20743,7 @@
         <v>105</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>3795</v>
+        <v>3794</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>1766</v>
@@ -22481,13 +22481,13 @@
         <v>1</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>3536</v>
+        <v>3535</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>3536</v>
+        <v>3535</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>3535</v>
+        <v>3534</v>
       </c>
       <c r="F129" s="2" t="s">
         <v>72</v>
@@ -22496,19 +22496,19 @@
         <v>38884</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>3534</v>
+        <v>3533</v>
       </c>
       <c r="I129" s="2" t="s">
-        <v>3533</v>
+        <v>3532</v>
       </c>
       <c r="J129" s="2" t="s">
-        <v>3532</v>
+        <v>3531</v>
       </c>
       <c r="K129" s="2">
         <v>316.15690000000001</v>
       </c>
       <c r="L129" s="2" t="s">
-        <v>3531</v>
+        <v>3530</v>
       </c>
       <c r="M129" s="2">
         <v>0</v>
@@ -22549,7 +22549,7 @@
         <v>380</v>
       </c>
       <c r="AA129" s="2" t="s">
-        <v>3530</v>
+        <v>3529</v>
       </c>
       <c r="AB129" s="2"/>
       <c r="AC129" s="2"/>
@@ -23267,13 +23267,13 @@
         <v>1</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>3520</v>
+        <v>3519</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>3520</v>
+        <v>3519</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>3519</v>
+        <v>3518</v>
       </c>
       <c r="F139" s="2" t="s">
         <v>84</v>
@@ -23282,19 +23282,19 @@
         <v>931</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>3518</v>
+        <v>3517</v>
       </c>
       <c r="I139" s="2" t="s">
-        <v>3517</v>
+        <v>3516</v>
       </c>
       <c r="J139" s="2" t="s">
-        <v>3516</v>
+        <v>3515</v>
       </c>
       <c r="K139" s="2">
         <v>128.0626</v>
       </c>
       <c r="L139" s="2" t="s">
-        <v>3515</v>
+        <v>3514</v>
       </c>
       <c r="M139" s="2">
         <v>0.1</v>
@@ -23303,7 +23303,7 @@
         <v>97</v>
       </c>
       <c r="O139" s="2" t="s">
-        <v>3514</v>
+        <v>3513</v>
       </c>
       <c r="P139" s="2" t="s">
         <v>14</v>
@@ -23425,13 +23425,13 @@
         <v>1</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>3570</v>
+        <v>3569</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>3570</v>
+        <v>3569</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>3569</v>
+        <v>3568</v>
       </c>
       <c r="F141" s="2" t="s">
         <v>25</v>
@@ -23440,19 +23440,19 @@
         <v>7242</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>3568</v>
+        <v>3567</v>
       </c>
       <c r="I141" s="2" t="s">
-        <v>3567</v>
+        <v>3566</v>
       </c>
       <c r="J141" s="2" t="s">
-        <v>3566</v>
+        <v>3565</v>
       </c>
       <c r="K141" s="2">
         <v>107.0735</v>
       </c>
       <c r="L141" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="M141" s="2">
         <v>6.6666666999999999E-2</v>
@@ -23461,7 +23461,7 @@
         <v>97</v>
       </c>
       <c r="O141" s="2" t="s">
-        <v>3564</v>
+        <v>3563</v>
       </c>
       <c r="P141" s="2">
         <v>1</v>
@@ -23587,7 +23587,7 @@
         <v>1</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>3833</v>
+        <v>3832</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>2383</v>
@@ -23745,10 +23745,10 @@
         <v>105</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>3856</v>
+        <v>3855</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>3856</v>
+        <v>3855</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>2616</v>
@@ -23823,7 +23823,7 @@
         <v>105</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>3857</v>
+        <v>3856</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>467</v>
@@ -23981,10 +23981,10 @@
         <v>105</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>3861</v>
+        <v>3860</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>3861</v>
+        <v>3860</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>815</v>
@@ -24613,13 +24613,13 @@
         <v>1</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>3575</v>
+        <v>3574</v>
       </c>
       <c r="F156" s="2" t="s">
         <v>62</v>
@@ -24628,19 +24628,19 @@
         <v>7000</v>
       </c>
       <c r="H156" s="2" t="s">
-        <v>3574</v>
+        <v>3573</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>3573</v>
+        <v>3572</v>
       </c>
       <c r="J156" s="2" t="s">
-        <v>3572</v>
+        <v>3571</v>
       </c>
       <c r="K156" s="2">
         <v>123.0684</v>
       </c>
       <c r="L156" s="2" t="s">
-        <v>3571</v>
+        <v>3570</v>
       </c>
       <c r="M156" s="2">
         <v>0.45</v>
@@ -25089,7 +25089,7 @@
         <v>1</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>3791</v>
+        <v>3790</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>2523</v>
@@ -25169,7 +25169,7 @@
         <v>105</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>3792</v>
+        <v>3791</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>1802</v>
@@ -25249,7 +25249,7 @@
         <v>105</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>3793</v>
+        <v>3792</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>1795</v>
@@ -25329,10 +25329,10 @@
         <v>105</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>3770</v>
+        <v>3769</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>3770</v>
+        <v>3769</v>
       </c>
       <c r="E165" s="2" t="s">
         <v>1772</v>
@@ -25957,10 +25957,10 @@
         <v>105</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>3767</v>
+        <v>3766</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>3767</v>
+        <v>3766</v>
       </c>
       <c r="E173" s="2" t="s">
         <v>1461</v>
@@ -26597,7 +26597,7 @@
         <v>105</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>3843</v>
+        <v>3842</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>238</v>
@@ -26675,10 +26675,10 @@
         <v>105</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>3854</v>
+        <v>3853</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>3854</v>
+        <v>3853</v>
       </c>
       <c r="E182" s="2" t="s">
         <v>922</v>
@@ -27215,13 +27215,13 @@
         <v>1</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>3563</v>
+        <v>3562</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>3563</v>
+        <v>3562</v>
       </c>
       <c r="E189" s="2" t="s">
-        <v>3562</v>
+        <v>3561</v>
       </c>
       <c r="F189" s="2" t="s">
         <v>65</v>
@@ -27230,13 +27230,13 @@
         <v>4115</v>
       </c>
       <c r="H189" s="2" t="s">
-        <v>3561</v>
+        <v>3560</v>
       </c>
       <c r="I189" s="2" t="s">
-        <v>3560</v>
+        <v>3559</v>
       </c>
       <c r="J189" s="2" t="s">
-        <v>3559</v>
+        <v>3558</v>
       </c>
       <c r="K189" s="2">
         <v>344.0138</v>
@@ -27251,7 +27251,7 @@
         <v>97</v>
       </c>
       <c r="O189" s="2" t="s">
-        <v>3558</v>
+        <v>3557</v>
       </c>
       <c r="P189" s="2">
         <v>3</v>
@@ -27609,10 +27609,10 @@
         <v>105</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>3476</v>
+        <v>3896</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>3476</v>
+        <v>3896</v>
       </c>
       <c r="E194" s="2" t="s">
         <v>3475</v>
@@ -27691,7 +27691,7 @@
         <v>105</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>3796</v>
+        <v>3795</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>1689</v>
@@ -27849,7 +27849,7 @@
         <v>105</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>3807</v>
+        <v>3806</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>1560</v>
@@ -28239,10 +28239,10 @@
         <v>1</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>3687</v>
+        <v>3686</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>3687</v>
+        <v>3686</v>
       </c>
       <c r="E202" s="2" t="s">
         <v>2425</v>
@@ -28631,7 +28631,7 @@
         <v>105</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>3836</v>
+        <v>3835</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>419</v>
@@ -28787,10 +28787,10 @@
         <v>105</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>3850</v>
+        <v>3849</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>3850</v>
+        <v>3849</v>
       </c>
       <c r="E209" s="2" t="s">
         <v>1301</v>
@@ -29413,10 +29413,10 @@
         <v>105</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>3882</v>
+        <v>3881</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>3882</v>
+        <v>3881</v>
       </c>
       <c r="E217" s="2" t="s">
         <v>545</v>
@@ -29497,10 +29497,10 @@
         <v>105</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>3883</v>
+        <v>3882</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>3883</v>
+        <v>3882</v>
       </c>
       <c r="E218" s="2" t="s">
         <v>1839</v>
@@ -29893,7 +29893,7 @@
         <v>105</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>3806</v>
+        <v>3805</v>
       </c>
       <c r="D223" s="2" t="s">
         <v>2736</v>
@@ -30357,7 +30357,7 @@
         <v>1</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>3808</v>
+        <v>3807</v>
       </c>
       <c r="D229" s="2" t="s">
         <v>49</v>
@@ -30979,28 +30979,28 @@
         <v>105</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>3500</v>
+        <v>3499</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>3500</v>
+        <v>3499</v>
       </c>
       <c r="E237" s="2" t="s">
-        <v>3499</v>
+        <v>3498</v>
       </c>
       <c r="F237" s="2" t="s">
-        <v>3498</v>
+        <v>3497</v>
       </c>
       <c r="G237" s="2">
         <v>7057</v>
       </c>
       <c r="H237" s="2" t="s">
-        <v>3497</v>
+        <v>3496</v>
       </c>
       <c r="I237" s="2" t="s">
-        <v>3496</v>
+        <v>3495</v>
       </c>
       <c r="J237" s="2" t="s">
-        <v>3495</v>
+        <v>3494</v>
       </c>
       <c r="K237" s="2">
         <v>143.0735</v>
@@ -31015,7 +31015,7 @@
         <v>97</v>
       </c>
       <c r="O237" s="2" t="s">
-        <v>3494</v>
+        <v>3493</v>
       </c>
       <c r="P237" s="2">
         <v>1</v>
@@ -31055,7 +31055,7 @@
         <v>105</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>3774</v>
+        <v>3773</v>
       </c>
       <c r="D238" s="2" t="s">
         <v>3284</v>
@@ -31289,7 +31289,7 @@
         <v>105</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>3788</v>
+        <v>3787</v>
       </c>
       <c r="D241" s="2" t="s">
         <v>1855</v>
@@ -31367,7 +31367,7 @@
         <v>1</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>3797</v>
+        <v>3796</v>
       </c>
       <c r="D242" s="2" t="s">
         <v>2501</v>
@@ -31447,7 +31447,7 @@
         <v>105</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>3798</v>
+        <v>3797</v>
       </c>
       <c r="D243" s="2" t="s">
         <v>3164</v>
@@ -31837,10 +31837,10 @@
         <v>105</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>3768</v>
+        <v>3767</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>3768</v>
+        <v>3767</v>
       </c>
       <c r="E248" s="2" t="s">
         <v>1252</v>
@@ -32155,7 +32155,7 @@
         <v>105</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>3872</v>
+        <v>3871</v>
       </c>
       <c r="D252" s="2" t="s">
         <v>2601</v>
@@ -32239,34 +32239,34 @@
         <v>105</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>3772</v>
+        <v>3771</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>3507</v>
+        <v>3506</v>
       </c>
       <c r="E253" s="2" t="s">
-        <v>3506</v>
+        <v>3505</v>
       </c>
       <c r="F253" s="2" t="s">
-        <v>3505</v>
+        <v>3504</v>
       </c>
       <c r="G253" s="2">
         <v>7015</v>
       </c>
       <c r="H253" s="2" t="s">
-        <v>3504</v>
+        <v>3503</v>
       </c>
       <c r="I253" s="2" t="s">
-        <v>3503</v>
+        <v>3502</v>
       </c>
       <c r="J253" s="2" t="s">
-        <v>3502</v>
+        <v>3501</v>
       </c>
       <c r="K253" s="2">
         <v>169.08920000000001</v>
       </c>
       <c r="L253" s="2" t="s">
-        <v>3501</v>
+        <v>3500</v>
       </c>
       <c r="M253" s="2">
         <v>0.46666666699999998</v>
@@ -32317,34 +32317,34 @@
         <v>105</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>3780</v>
+        <v>3779</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>3493</v>
+        <v>3492</v>
       </c>
       <c r="E254" s="2" t="s">
-        <v>3492</v>
+        <v>3491</v>
       </c>
       <c r="F254" s="2" t="s">
-        <v>3491</v>
+        <v>3490</v>
       </c>
       <c r="G254" s="2">
         <v>7102</v>
       </c>
       <c r="H254" s="2" t="s">
-        <v>3490</v>
+        <v>3489</v>
       </c>
       <c r="I254" s="2" t="s">
-        <v>3489</v>
+        <v>3488</v>
       </c>
       <c r="J254" s="2" t="s">
-        <v>3488</v>
+        <v>3487</v>
       </c>
       <c r="K254" s="2">
         <v>169.0891</v>
       </c>
       <c r="L254" s="2" t="s">
-        <v>3487</v>
+        <v>3486</v>
       </c>
       <c r="M254" s="2">
         <v>0.51666666699999997</v>
@@ -32353,7 +32353,7 @@
         <v>97</v>
       </c>
       <c r="O254" s="2" t="s">
-        <v>3486</v>
+        <v>3485</v>
       </c>
       <c r="P254" s="2">
         <v>1</v>
@@ -32547,7 +32547,7 @@
         <v>1</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>3809</v>
+        <v>3808</v>
       </c>
       <c r="D257" s="2" t="s">
         <v>2471</v>
@@ -32625,10 +32625,10 @@
         <v>105</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>3769</v>
+        <v>3768</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>3769</v>
+        <v>3768</v>
       </c>
       <c r="E258" s="2" t="s">
         <v>1246</v>
@@ -32863,7 +32863,7 @@
         <v>105</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>3841</v>
+        <v>3840</v>
       </c>
       <c r="D261" s="2" t="s">
         <v>3015</v>
@@ -33571,13 +33571,13 @@
         <v>1</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>3619</v>
+        <v>3618</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>3619</v>
+        <v>3618</v>
       </c>
       <c r="E270" s="2" t="s">
-        <v>3618</v>
+        <v>3617</v>
       </c>
       <c r="F270" s="2" t="s">
         <v>51</v>
@@ -33586,19 +33586,19 @@
         <v>5954</v>
       </c>
       <c r="H270" s="2" t="s">
-        <v>3617</v>
+        <v>3616</v>
       </c>
       <c r="I270" s="2" t="s">
-        <v>3616</v>
+        <v>3615</v>
       </c>
       <c r="J270" s="2" t="s">
-        <v>3615</v>
+        <v>3614</v>
       </c>
       <c r="K270" s="2">
         <v>228.09389999999999</v>
       </c>
       <c r="L270" s="2" t="s">
-        <v>3614</v>
+        <v>3613</v>
       </c>
       <c r="M270" s="2">
         <v>0.133333333</v>
@@ -33607,7 +33607,7 @@
         <v>97</v>
       </c>
       <c r="O270" s="2" t="s">
-        <v>3613</v>
+        <v>3612</v>
       </c>
       <c r="P270" s="2" t="s">
         <v>14</v>
@@ -33809,13 +33809,13 @@
         <v>1</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>3826</v>
+        <v>3825</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>3598</v>
+        <v>3597</v>
       </c>
       <c r="E273" s="2" t="s">
-        <v>3597</v>
+        <v>3596</v>
       </c>
       <c r="F273" s="2" t="s">
         <v>77</v>
@@ -33824,13 +33824,13 @@
         <v>7340</v>
       </c>
       <c r="H273" s="2" t="s">
-        <v>3596</v>
+        <v>3595</v>
       </c>
       <c r="I273" s="2" t="s">
-        <v>3595</v>
+        <v>3594</v>
       </c>
       <c r="J273" s="2" t="s">
-        <v>3594</v>
+        <v>3593</v>
       </c>
       <c r="K273" s="2">
         <v>225.1266</v>
@@ -33965,13 +33965,13 @@
         <v>1</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>3625</v>
+        <v>3624</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>3625</v>
+        <v>3624</v>
       </c>
       <c r="E275" s="2" t="s">
-        <v>3624</v>
+        <v>3623</v>
       </c>
       <c r="F275" s="2" t="s">
         <v>40</v>
@@ -33980,19 +33980,19 @@
         <v>7579</v>
       </c>
       <c r="H275" s="2" t="s">
-        <v>3623</v>
+        <v>3622</v>
       </c>
       <c r="I275" s="2" t="s">
-        <v>3622</v>
+        <v>3621</v>
       </c>
       <c r="J275" s="2" t="s">
-        <v>3621</v>
+        <v>3620</v>
       </c>
       <c r="K275" s="2">
         <v>200.09495999999999</v>
       </c>
       <c r="L275" s="2" t="s">
-        <v>3620</v>
+        <v>3619</v>
       </c>
       <c r="M275" s="2">
         <v>0</v>
@@ -34195,10 +34195,10 @@
         <v>105</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>3864</v>
+        <v>3863</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>3864</v>
+        <v>3863</v>
       </c>
       <c r="E278" s="2" t="s">
         <v>628</v>
@@ -34669,10 +34669,10 @@
         <v>105</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>3881</v>
+        <v>3880</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>3881</v>
+        <v>3880</v>
       </c>
       <c r="E284" s="2" t="s">
         <v>3359</v>
@@ -35063,7 +35063,7 @@
         <v>105</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>3782</v>
+        <v>3781</v>
       </c>
       <c r="D289" s="2" t="s">
         <v>2018</v>
@@ -35141,7 +35141,7 @@
         <v>105</v>
       </c>
       <c r="C290" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="D290" s="2" t="s">
         <v>1624</v>
@@ -35221,7 +35221,7 @@
         <v>105</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>3810</v>
+        <v>3809</v>
       </c>
       <c r="D291" s="2" t="s">
         <v>2720</v>
@@ -35461,7 +35461,7 @@
         <v>105</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="D294" s="2" t="s">
         <v>1159</v>
@@ -35861,7 +35861,7 @@
         <v>105</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>3858</v>
+        <v>3857</v>
       </c>
       <c r="D299" s="2" t="s">
         <v>213</v>
@@ -36019,34 +36019,34 @@
         <v>1</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>3655</v>
+        <v>3654</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>3654</v>
+        <v>3653</v>
       </c>
       <c r="E301" s="2" t="s">
-        <v>3653</v>
+        <v>3652</v>
       </c>
       <c r="F301" s="2" t="s">
-        <v>3652</v>
+        <v>3651</v>
       </c>
       <c r="G301" s="2">
         <v>8765</v>
       </c>
       <c r="H301" s="2" t="s">
-        <v>3651</v>
+        <v>3650</v>
       </c>
       <c r="I301" s="2" t="s">
-        <v>3650</v>
+        <v>3649</v>
       </c>
       <c r="J301" s="2" t="s">
-        <v>3649</v>
+        <v>3648</v>
       </c>
       <c r="K301" s="2">
         <v>216.07210000000001</v>
       </c>
       <c r="L301" s="2" t="s">
-        <v>3648</v>
+        <v>3647</v>
       </c>
       <c r="M301" s="2">
         <v>0</v>
@@ -36085,7 +36085,7 @@
         <v>1160</v>
       </c>
       <c r="AA301" s="2" t="s">
-        <v>3647</v>
+        <v>3646</v>
       </c>
       <c r="AB301" s="2"/>
       <c r="AC301" s="2"/>
@@ -36255,7 +36255,7 @@
         <v>105</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>3868</v>
+        <v>3867</v>
       </c>
       <c r="D304" s="2" t="s">
         <v>1779</v>
@@ -36569,10 +36569,10 @@
         <v>105</v>
       </c>
       <c r="C308" s="2" t="s">
-        <v>3884</v>
+        <v>3883</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>3884</v>
+        <v>3883</v>
       </c>
       <c r="E308" s="2" t="s">
         <v>2884</v>
@@ -36732,7 +36732,7 @@
         <v>798</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>3893</v>
+        <v>3892</v>
       </c>
       <c r="E310" s="2" t="s">
         <v>797</v>
@@ -36881,7 +36881,7 @@
         <v>105</v>
       </c>
       <c r="C312" s="2" t="s">
-        <v>3804</v>
+        <v>3803</v>
       </c>
       <c r="D312" s="2" t="s">
         <v>1610</v>
@@ -36959,7 +36959,7 @@
         <v>105</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>3805</v>
+        <v>3804</v>
       </c>
       <c r="D313" s="2" t="s">
         <v>1602</v>
@@ -37039,16 +37039,16 @@
         <v>1</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>3896</v>
+        <v>3895</v>
       </c>
       <c r="D314" s="2" t="s">
-        <v>3894</v>
+        <v>3893</v>
       </c>
       <c r="E314" s="2" t="s">
         <v>2388</v>
       </c>
       <c r="F314" s="2" t="s">
-        <v>3895</v>
+        <v>3894</v>
       </c>
       <c r="G314" s="2">
         <v>42851</v>
@@ -37117,7 +37117,7 @@
         <v>105</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>3832</v>
+        <v>3831</v>
       </c>
       <c r="D315" s="2" t="s">
         <v>534</v>
@@ -37193,7 +37193,7 @@
         <v>105</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>3844</v>
+        <v>3843</v>
       </c>
       <c r="D316" s="2" t="s">
         <v>182</v>
@@ -37427,10 +37427,10 @@
         <v>1</v>
       </c>
       <c r="C319" s="2" t="s">
-        <v>3863</v>
+        <v>3862</v>
       </c>
       <c r="D319" s="2" t="s">
-        <v>3863</v>
+        <v>3862</v>
       </c>
       <c r="E319" s="2" t="s">
         <v>2548</v>
@@ -37503,7 +37503,7 @@
         <v>105</v>
       </c>
       <c r="C320" s="2" t="s">
-        <v>3869</v>
+        <v>3868</v>
       </c>
       <c r="D320" s="2" t="s">
         <v>190</v>
@@ -37581,7 +37581,7 @@
         <v>105</v>
       </c>
       <c r="C321" s="2" t="s">
-        <v>3871</v>
+        <v>3870</v>
       </c>
       <c r="D321" s="2" t="s">
         <v>175</v>
@@ -38053,13 +38053,13 @@
         <v>1</v>
       </c>
       <c r="C327" s="2" t="s">
-        <v>3786</v>
+        <v>3785</v>
       </c>
       <c r="D327" s="2" t="s">
-        <v>3513</v>
+        <v>3512</v>
       </c>
       <c r="E327" s="2" t="s">
-        <v>3512</v>
+        <v>3511</v>
       </c>
       <c r="F327" s="2" t="s">
         <v>52</v>
@@ -38068,19 +38068,19 @@
         <v>7444</v>
       </c>
       <c r="H327" s="2" t="s">
-        <v>3511</v>
+        <v>3510</v>
       </c>
       <c r="I327" s="2" t="s">
-        <v>3510</v>
+        <v>3509</v>
       </c>
       <c r="J327" s="2" t="s">
-        <v>3509</v>
+        <v>3508</v>
       </c>
       <c r="K327" s="2">
         <v>152.05860000000001</v>
       </c>
       <c r="L327" s="2" t="s">
-        <v>3508</v>
+        <v>3507</v>
       </c>
       <c r="M327" s="2">
         <v>0.15</v>
@@ -38213,13 +38213,13 @@
         <v>1</v>
       </c>
       <c r="C329" s="2" t="s">
-        <v>3612</v>
+        <v>3611</v>
       </c>
       <c r="D329" s="2" t="s">
-        <v>3612</v>
+        <v>3611</v>
       </c>
       <c r="E329" s="2" t="s">
-        <v>3611</v>
+        <v>3610</v>
       </c>
       <c r="F329" s="2" t="s">
         <v>61</v>
@@ -38228,13 +38228,13 @@
         <v>9158</v>
       </c>
       <c r="H329" s="2" t="s">
-        <v>3610</v>
+        <v>3609</v>
       </c>
       <c r="I329" s="2" t="s">
-        <v>3609</v>
+        <v>3608</v>
       </c>
       <c r="J329" s="2" t="s">
-        <v>3608</v>
+        <v>3607</v>
       </c>
       <c r="K329" s="2">
         <v>252.09389999999999</v>
@@ -38249,7 +38249,7 @@
         <v>97</v>
       </c>
       <c r="O329" s="2" t="s">
-        <v>3607</v>
+        <v>3606</v>
       </c>
       <c r="P329" s="2" t="s">
         <v>14</v>
@@ -38295,7 +38295,7 @@
         <v>105</v>
       </c>
       <c r="C330" s="2" t="s">
-        <v>3812</v>
+        <v>3811</v>
       </c>
       <c r="D330" s="2" t="s">
         <v>3114</v>
@@ -38379,7 +38379,7 @@
         <v>105</v>
       </c>
       <c r="C331" s="2" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="D331" s="2" t="s">
         <v>1119</v>
@@ -38457,7 +38457,7 @@
         <v>105</v>
       </c>
       <c r="C332" s="2" t="s">
-        <v>3824</v>
+        <v>3823</v>
       </c>
       <c r="D332" s="2" t="s">
         <v>2649</v>
@@ -38535,7 +38535,7 @@
         <v>105</v>
       </c>
       <c r="C333" s="2" t="s">
-        <v>3831</v>
+        <v>3830</v>
       </c>
       <c r="D333" s="2" t="s">
         <v>612</v>
@@ -38613,7 +38613,7 @@
         <v>105</v>
       </c>
       <c r="C334" s="2" t="s">
-        <v>3834</v>
+        <v>3833</v>
       </c>
       <c r="D334" s="2" t="s">
         <v>525</v>
@@ -38691,7 +38691,7 @@
         <v>105</v>
       </c>
       <c r="C335" s="2" t="s">
-        <v>3860</v>
+        <v>3859</v>
       </c>
       <c r="D335" s="2" t="s">
         <v>301</v>
@@ -38847,13 +38847,13 @@
         <v>1</v>
       </c>
       <c r="C337" s="2" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
       <c r="D337" s="2" t="s">
-        <v>3556</v>
+        <v>3555</v>
       </c>
       <c r="E337" s="2" t="s">
-        <v>3555</v>
+        <v>3554</v>
       </c>
       <c r="F337" s="2" t="s">
         <v>28</v>
@@ -38862,19 +38862,19 @@
         <v>6359</v>
       </c>
       <c r="H337" s="2" t="s">
-        <v>3554</v>
+        <v>3553</v>
       </c>
       <c r="I337" s="2" t="s">
-        <v>3553</v>
+        <v>3552</v>
       </c>
       <c r="J337" s="2" t="s">
-        <v>3552</v>
+        <v>3551</v>
       </c>
       <c r="K337" s="2">
         <v>161.8639</v>
       </c>
       <c r="L337" s="2" t="s">
-        <v>3551</v>
+        <v>3550</v>
       </c>
       <c r="M337" s="2">
         <v>0</v>
@@ -39079,7 +39079,7 @@
         <v>105</v>
       </c>
       <c r="C340" s="2" t="s">
-        <v>3776</v>
+        <v>3775</v>
       </c>
       <c r="D340" s="2" t="s">
         <v>2155</v>
@@ -39159,7 +39159,7 @@
         <v>105</v>
       </c>
       <c r="C341" s="2" t="s">
-        <v>3777</v>
+        <v>3776</v>
       </c>
       <c r="D341" s="2" t="s">
         <v>2144</v>
@@ -39237,7 +39237,7 @@
         <v>105</v>
       </c>
       <c r="C342" s="2" t="s">
-        <v>3781</v>
+        <v>3780</v>
       </c>
       <c r="D342" s="2" t="s">
         <v>2999</v>
@@ -39395,7 +39395,7 @@
         <v>1</v>
       </c>
       <c r="C344" s="2" t="s">
-        <v>3799</v>
+        <v>3798</v>
       </c>
       <c r="D344" s="2" t="s">
         <v>2494</v>
@@ -39475,7 +39475,7 @@
         <v>1</v>
       </c>
       <c r="C345" s="2" t="s">
-        <v>3800</v>
+        <v>3799</v>
       </c>
       <c r="D345" s="2" t="s">
         <v>2488</v>
@@ -39555,7 +39555,7 @@
         <v>105</v>
       </c>
       <c r="C346" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="D346" s="2" t="s">
         <v>3148</v>
@@ -39633,7 +39633,7 @@
         <v>105</v>
       </c>
       <c r="C347" s="2" t="s">
-        <v>3818</v>
+        <v>3817</v>
       </c>
       <c r="D347" s="2" t="s">
         <v>1097</v>
@@ -39711,7 +39711,7 @@
         <v>105</v>
       </c>
       <c r="C348" s="2" t="s">
-        <v>3865</v>
+        <v>3864</v>
       </c>
       <c r="D348" s="2" t="s">
         <v>1134</v>
@@ -40343,7 +40343,7 @@
         <v>105</v>
       </c>
       <c r="C356" s="2" t="s">
-        <v>3819</v>
+        <v>3818</v>
       </c>
       <c r="D356" s="2" t="s">
         <v>1089</v>
@@ -40423,7 +40423,7 @@
         <v>105</v>
       </c>
       <c r="C357" s="2" t="s">
-        <v>3820</v>
+        <v>3819</v>
       </c>
       <c r="D357" s="2" t="s">
         <v>1081</v>
@@ -40503,7 +40503,7 @@
         <v>105</v>
       </c>
       <c r="C358" s="2" t="s">
-        <v>3823</v>
+        <v>3822</v>
       </c>
       <c r="D358" s="2" t="s">
         <v>2936</v>
@@ -40581,7 +40581,7 @@
         <v>105</v>
       </c>
       <c r="C359" s="2" t="s">
-        <v>3830</v>
+        <v>3829</v>
       </c>
       <c r="D359" s="2" t="s">
         <v>702</v>
@@ -40657,7 +40657,7 @@
         <v>1</v>
       </c>
       <c r="C360" s="2" t="s">
-        <v>3839</v>
+        <v>3838</v>
       </c>
       <c r="D360" s="2" t="s">
         <v>35</v>
@@ -40733,7 +40733,7 @@
         <v>105</v>
       </c>
       <c r="C361" s="2" t="s">
-        <v>3840</v>
+        <v>3839</v>
       </c>
       <c r="D361" s="2" t="s">
         <v>330</v>
@@ -40891,7 +40891,7 @@
         <v>105</v>
       </c>
       <c r="C363" s="2" t="s">
-        <v>3870</v>
+        <v>3869</v>
       </c>
       <c r="D363" s="2" t="s">
         <v>196</v>
@@ -41205,13 +41205,13 @@
         <v>1</v>
       </c>
       <c r="C367" s="2" t="s">
-        <v>3779</v>
+        <v>3778</v>
       </c>
       <c r="D367" s="2" t="s">
-        <v>3638</v>
+        <v>3637</v>
       </c>
       <c r="E367" s="2" t="s">
-        <v>3637</v>
+        <v>3636</v>
       </c>
       <c r="F367" s="2" t="s">
         <v>76</v>
@@ -41220,19 +41220,19 @@
         <v>8413</v>
       </c>
       <c r="H367" s="2" t="s">
-        <v>3636</v>
+        <v>3635</v>
       </c>
       <c r="I367" s="2" t="s">
-        <v>3635</v>
+        <v>3634</v>
       </c>
       <c r="J367" s="2" t="s">
-        <v>3634</v>
+        <v>3633</v>
       </c>
       <c r="K367" s="2">
         <v>212.13140000000001</v>
       </c>
       <c r="L367" s="2" t="s">
-        <v>3633</v>
+        <v>3632</v>
       </c>
       <c r="M367" s="2">
         <v>0</v>
@@ -41369,7 +41369,7 @@
         <v>105</v>
       </c>
       <c r="C369" s="2" t="s">
-        <v>3794</v>
+        <v>3793</v>
       </c>
       <c r="D369" s="2" t="s">
         <v>3220</v>
@@ -41451,7 +41451,7 @@
         <v>105</v>
       </c>
       <c r="C370" s="2" t="s">
-        <v>3817</v>
+        <v>3816</v>
       </c>
       <c r="D370" s="2" t="s">
         <v>1111</v>
@@ -41529,7 +41529,7 @@
         <v>105</v>
       </c>
       <c r="C371" s="2" t="s">
-        <v>3827</v>
+        <v>3826</v>
       </c>
       <c r="D371" s="2" t="s">
         <v>885</v>
@@ -41603,7 +41603,7 @@
         <v>105</v>
       </c>
       <c r="C372" s="2" t="s">
-        <v>3842</v>
+        <v>3841</v>
       </c>
       <c r="D372" s="2" t="s">
         <v>275</v>
@@ -41685,7 +41685,7 @@
         <v>105</v>
       </c>
       <c r="C373" s="2" t="s">
-        <v>3846</v>
+        <v>3845</v>
       </c>
       <c r="D373" s="2" t="s">
         <v>133</v>
@@ -41765,7 +41765,7 @@
         <v>1</v>
       </c>
       <c r="C374" s="2" t="s">
-        <v>3846</v>
+        <v>3845</v>
       </c>
       <c r="D374" s="2" t="s">
         <v>37</v>
@@ -41923,7 +41923,7 @@
         <v>105</v>
       </c>
       <c r="C376" s="2" t="s">
-        <v>3848</v>
+        <v>3847</v>
       </c>
       <c r="D376" s="2" t="s">
         <v>1104</v>
@@ -42001,7 +42001,7 @@
         <v>105</v>
       </c>
       <c r="C377" s="2" t="s">
-        <v>3851</v>
+        <v>3850</v>
       </c>
       <c r="D377" s="2" t="s">
         <v>3229</v>
@@ -42465,7 +42465,7 @@
         <v>105</v>
       </c>
       <c r="C383" s="2" t="s">
-        <v>3778</v>
+        <v>3777</v>
       </c>
       <c r="D383" s="2" t="s">
         <v>2820</v>
@@ -42623,34 +42623,34 @@
         <v>1</v>
       </c>
       <c r="C385" s="2" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="D385" s="2" t="s">
-        <v>3529</v>
+        <v>3528</v>
       </c>
       <c r="E385" s="2" t="s">
-        <v>3528</v>
+        <v>3527</v>
       </c>
       <c r="F385" s="2" t="s">
-        <v>3527</v>
+        <v>3526</v>
       </c>
       <c r="G385" s="2">
         <v>4156</v>
       </c>
       <c r="H385" s="2" t="s">
-        <v>3526</v>
+        <v>3525</v>
       </c>
       <c r="I385" s="2" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="J385" s="2" t="s">
-        <v>3524</v>
+        <v>3523</v>
       </c>
       <c r="K385" s="2">
         <v>110.00369999999999</v>
       </c>
       <c r="L385" s="2" t="s">
-        <v>3523</v>
+        <v>3522</v>
       </c>
       <c r="M385" s="2">
         <v>0</v>
@@ -42665,7 +42665,7 @@
         <v>64</v>
       </c>
       <c r="Q385" s="2" t="s">
-        <v>3522</v>
+        <v>3521</v>
       </c>
       <c r="R385" s="2"/>
       <c r="S385" s="2" t="s">
@@ -42687,7 +42687,7 @@
         <v>1978</v>
       </c>
       <c r="AA385" s="2" t="s">
-        <v>3521</v>
+        <v>3520</v>
       </c>
       <c r="AB385" s="2"/>
       <c r="AC385" s="2"/>
@@ -42777,7 +42777,7 @@
         <v>105</v>
       </c>
       <c r="C387" s="2" t="s">
-        <v>3828</v>
+        <v>3827</v>
       </c>
       <c r="D387" s="2" t="s">
         <v>859</v>
@@ -42931,13 +42931,13 @@
         <v>1</v>
       </c>
       <c r="C389" s="2" t="s">
-        <v>3586</v>
+        <v>3585</v>
       </c>
       <c r="D389" s="2" t="s">
-        <v>3585</v>
+        <v>3584</v>
       </c>
       <c r="E389" s="2" t="s">
-        <v>3584</v>
+        <v>3583</v>
       </c>
       <c r="F389" s="2" t="s">
         <v>56</v>
@@ -42946,19 +42946,19 @@
         <v>5955</v>
       </c>
       <c r="H389" s="2" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="I389" s="2" t="s">
-        <v>3582</v>
+        <v>3581</v>
       </c>
       <c r="J389" s="2" t="s">
-        <v>3581</v>
+        <v>3580</v>
       </c>
       <c r="K389" s="2">
         <v>190.0378</v>
       </c>
       <c r="L389" s="2" t="s">
-        <v>3580</v>
+        <v>3579</v>
       </c>
       <c r="M389" s="2">
         <v>0</v>
@@ -42987,13 +42987,13 @@
       </c>
       <c r="X389" s="3"/>
       <c r="Y389" s="2" t="s">
-        <v>3579</v>
+        <v>3578</v>
       </c>
       <c r="Z389" s="2" t="s">
-        <v>3578</v>
+        <v>3577</v>
       </c>
       <c r="AA389" s="2" t="s">
-        <v>3577</v>
+        <v>3576</v>
       </c>
       <c r="AB389" s="2"/>
       <c r="AC389" s="2"/>
@@ -43083,7 +43083,7 @@
         <v>105</v>
       </c>
       <c r="C391" s="2" t="s">
-        <v>3785</v>
+        <v>3784</v>
       </c>
       <c r="D391" s="2" t="s">
         <v>2004</v>
@@ -43237,7 +43237,7 @@
         <v>105</v>
       </c>
       <c r="C393" s="2" t="s">
-        <v>3879</v>
+        <v>3878</v>
       </c>
       <c r="D393" s="2" t="s">
         <v>1126</v>
@@ -43315,7 +43315,7 @@
         <v>105</v>
       </c>
       <c r="C394" s="2" t="s">
-        <v>3790</v>
+        <v>3789</v>
       </c>
       <c r="D394" s="2" t="s">
         <v>2752</v>
@@ -43397,13 +43397,13 @@
         <v>1</v>
       </c>
       <c r="C395" s="2" t="s">
-        <v>3822</v>
+        <v>3821</v>
       </c>
       <c r="D395" s="2" t="s">
-        <v>3606</v>
+        <v>3605</v>
       </c>
       <c r="E395" s="2" t="s">
-        <v>3605</v>
+        <v>3604</v>
       </c>
       <c r="F395" s="2" t="s">
         <v>12</v>
@@ -43412,19 +43412,19 @@
         <v>12130</v>
       </c>
       <c r="H395" s="2" t="s">
-        <v>3604</v>
+        <v>3603</v>
       </c>
       <c r="I395" s="2" t="s">
-        <v>3603</v>
+        <v>3602</v>
       </c>
       <c r="J395" s="2" t="s">
-        <v>3602</v>
+        <v>3601</v>
       </c>
       <c r="K395" s="2">
         <v>130.11060000000001</v>
       </c>
       <c r="L395" s="2" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="M395" s="2">
         <v>0</v>
@@ -43433,7 +43433,7 @@
         <v>97</v>
       </c>
       <c r="O395" s="2" t="s">
-        <v>3600</v>
+        <v>3599</v>
       </c>
       <c r="P395" s="2" t="s">
         <v>14</v>
@@ -43446,7 +43446,7 @@
         <v>125</v>
       </c>
       <c r="T395" s="2" t="s">
-        <v>3599</v>
+        <v>3598</v>
       </c>
       <c r="U395" s="2"/>
       <c r="V395" s="2"/>
@@ -43553,7 +43553,7 @@
         <v>105</v>
       </c>
       <c r="C397" s="2" t="s">
-        <v>3829</v>
+        <v>3828</v>
       </c>
       <c r="D397" s="2" t="s">
         <v>2609</v>
@@ -43629,10 +43629,10 @@
         <v>105</v>
       </c>
       <c r="C398" s="2" t="s">
-        <v>3852</v>
+        <v>3851</v>
       </c>
       <c r="D398" s="2" t="s">
-        <v>3852</v>
+        <v>3851</v>
       </c>
       <c r="E398" s="2" t="s">
         <v>1810</v>
@@ -43705,7 +43705,7 @@
         <v>105</v>
       </c>
       <c r="C399" s="2" t="s">
-        <v>3853</v>
+        <v>3852</v>
       </c>
       <c r="D399" s="2" t="s">
         <v>876</v>
@@ -43939,7 +43939,7 @@
         <v>1</v>
       </c>
       <c r="C402" s="2" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="D402" s="2" t="s">
         <v>2420</v>
@@ -44019,10 +44019,10 @@
         <v>1</v>
       </c>
       <c r="C403" s="2" t="s">
-        <v>3825</v>
+        <v>3824</v>
       </c>
       <c r="D403" s="2" t="s">
-        <v>3686</v>
+        <v>3685</v>
       </c>
       <c r="E403" s="2" t="s">
         <v>2414</v>
@@ -44101,13 +44101,13 @@
         <v>1</v>
       </c>
       <c r="C404" s="2" t="s">
-        <v>3847</v>
+        <v>3846</v>
       </c>
       <c r="D404" s="2" t="s">
-        <v>3632</v>
+        <v>3631</v>
       </c>
       <c r="E404" s="2" t="s">
-        <v>3631</v>
+        <v>3630</v>
       </c>
       <c r="F404" s="2" t="s">
         <v>69</v>
@@ -44116,19 +44116,19 @@
         <v>7577</v>
       </c>
       <c r="H404" s="2" t="s">
-        <v>3630</v>
+        <v>3629</v>
       </c>
       <c r="I404" s="2" t="s">
-        <v>3629</v>
+        <v>3628</v>
       </c>
       <c r="J404" s="2" t="s">
-        <v>3628</v>
+        <v>3627</v>
       </c>
       <c r="K404" s="2">
         <v>198.1157</v>
       </c>
       <c r="L404" s="2" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
       <c r="M404" s="2">
         <v>0</v>
@@ -44137,7 +44137,7 @@
         <v>97</v>
       </c>
       <c r="O404" s="2" t="s">
-        <v>3626</v>
+        <v>3625</v>
       </c>
       <c r="P404" s="2" t="s">
         <v>14</v>
@@ -44183,7 +44183,7 @@
         <v>105</v>
       </c>
       <c r="C405" s="2" t="s">
-        <v>3849</v>
+        <v>3848</v>
       </c>
       <c r="D405" s="2" t="s">
         <v>266</v>
@@ -44497,7 +44497,7 @@
         <v>105</v>
       </c>
       <c r="C409" s="2" t="s">
-        <v>3801</v>
+        <v>3800</v>
       </c>
       <c r="D409" s="2" t="s">
         <v>2959</v>
@@ -44577,7 +44577,7 @@
         <v>105</v>
       </c>
       <c r="C410" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="D410" s="2" t="s">
         <v>1550</v>
@@ -44655,7 +44655,7 @@
         <v>105</v>
       </c>
       <c r="C411" s="2" t="s">
-        <v>3845</v>
+        <v>3844</v>
       </c>
       <c r="D411" s="2" t="s">
         <v>150</v>
@@ -44737,7 +44737,7 @@
         <v>105</v>
       </c>
       <c r="C412" s="2" t="s">
-        <v>3855</v>
+        <v>3854</v>
       </c>
       <c r="D412" s="2" t="s">
         <v>3008</v>
@@ -44821,7 +44821,7 @@
         <v>105</v>
       </c>
       <c r="C413" s="2" t="s">
-        <v>3773</v>
+        <v>3772</v>
       </c>
       <c r="D413" s="4" t="s">
         <v>2225</v>
@@ -45211,10 +45211,10 @@
         <v>105</v>
       </c>
       <c r="C418" s="2" t="s">
-        <v>3880</v>
+        <v>3879</v>
       </c>
       <c r="D418" s="2" t="s">
-        <v>3880</v>
+        <v>3879</v>
       </c>
       <c r="E418" s="2" t="s">
         <v>2064</v>
@@ -45365,7 +45365,7 @@
         <v>105</v>
       </c>
       <c r="C420" s="2" t="s">
-        <v>3789</v>
+        <v>3788</v>
       </c>
       <c r="D420" s="2" t="s">
         <v>3236</v>
@@ -45443,7 +45443,7 @@
         <v>1</v>
       </c>
       <c r="C421" s="2" t="s">
-        <v>3838</v>
+        <v>3837</v>
       </c>
       <c r="D421" s="2" t="s">
         <v>21</v>
@@ -45603,7 +45603,7 @@
         <v>105</v>
       </c>
       <c r="C423" s="2" t="s">
-        <v>3873</v>
+        <v>3872</v>
       </c>
       <c r="D423" s="2" t="s">
         <v>3301</v>
@@ -45687,34 +45687,34 @@
         <v>105</v>
       </c>
       <c r="C424" s="2" t="s">
-        <v>3485</v>
+        <v>3484</v>
       </c>
       <c r="D424" s="2" t="s">
-        <v>3484</v>
+        <v>3483</v>
       </c>
       <c r="E424" s="2" t="s">
-        <v>3483</v>
+        <v>3482</v>
       </c>
       <c r="F424" s="2" t="s">
-        <v>3482</v>
+        <v>3481</v>
       </c>
       <c r="G424" s="2">
         <v>7543</v>
       </c>
       <c r="H424" s="2" t="s">
-        <v>3481</v>
+        <v>3480</v>
       </c>
       <c r="I424" s="2" t="s">
-        <v>3480</v>
+        <v>3479</v>
       </c>
       <c r="J424" s="2" t="s">
-        <v>3479</v>
+        <v>3478</v>
       </c>
       <c r="K424" s="2">
         <v>266.03775000000002</v>
       </c>
       <c r="L424" s="2" t="s">
-        <v>3478</v>
+        <v>3477</v>
       </c>
       <c r="M424" s="2">
         <v>3.3333333E-2</v>
@@ -45723,7 +45723,7 @@
         <v>97</v>
       </c>
       <c r="O424" s="2" t="s">
-        <v>3477</v>
+        <v>3476</v>
       </c>
       <c r="P424" s="2">
         <v>1</v>
@@ -45765,7 +45765,7 @@
         <v>105</v>
       </c>
       <c r="C425" s="2" t="s">
-        <v>3866</v>
+        <v>3865</v>
       </c>
       <c r="D425" s="2" t="s">
         <v>2218</v>
@@ -45919,7 +45919,7 @@
         <v>105</v>
       </c>
       <c r="C427" s="2" t="s">
-        <v>3878</v>
+        <v>3877</v>
       </c>
       <c r="D427" s="2" t="s">
         <v>2316</v>
@@ -46157,7 +46157,7 @@
         <v>105</v>
       </c>
       <c r="C430" s="2" t="s">
-        <v>3837</v>
+        <v>3836</v>
       </c>
       <c r="D430" s="2" t="s">
         <v>358</v>
@@ -46391,7 +46391,7 @@
         <v>105</v>
       </c>
       <c r="C433" s="2" t="s">
-        <v>3775</v>
+        <v>3774</v>
       </c>
       <c r="D433" s="2" t="s">
         <v>2891</v>
@@ -46699,10 +46699,10 @@
         <v>105</v>
       </c>
       <c r="C437" s="2" t="s">
-        <v>3885</v>
+        <v>3884</v>
       </c>
       <c r="D437" s="2" t="s">
-        <v>3885</v>
+        <v>3884</v>
       </c>
       <c r="E437" s="2" t="s">
         <v>2251</v>
@@ -46855,10 +46855,10 @@
         <v>105</v>
       </c>
       <c r="C439" s="2" t="s">
+        <v>3873</v>
+      </c>
+      <c r="D439" s="2" t="s">
         <v>3874</v>
-      </c>
-      <c r="D439" s="2" t="s">
-        <v>3875</v>
       </c>
       <c r="E439" s="2" t="s">
         <v>1697</v>
@@ -47009,10 +47009,10 @@
         <v>1</v>
       </c>
       <c r="C441" s="2" t="s">
-        <v>3877</v>
+        <v>3876</v>
       </c>
       <c r="D441" s="2" t="s">
-        <v>3876</v>
+        <v>3875</v>
       </c>
       <c r="E441" s="2" t="s">
         <v>2350</v>
@@ -47163,7 +47163,7 @@
         <v>105</v>
       </c>
       <c r="C443" s="2" t="s">
-        <v>3867</v>
+        <v>3866</v>
       </c>
       <c r="D443" s="2" t="s">
         <v>1006</v>
@@ -47241,13 +47241,13 @@
         <v>1</v>
       </c>
       <c r="C444" s="2" t="s">
-        <v>3821</v>
+        <v>3820</v>
       </c>
       <c r="D444" s="2" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
       <c r="E444" s="2" t="s">
-        <v>3541</v>
+        <v>3540</v>
       </c>
       <c r="F444" s="2" t="s">
         <v>18</v>
@@ -47256,19 +47256,19 @@
         <v>22286931</v>
       </c>
       <c r="H444" s="2" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
       <c r="I444" s="2" t="s">
-        <v>3539</v>
+        <v>3538</v>
       </c>
       <c r="J444" s="2" t="s">
-        <v>3538</v>
+        <v>3537</v>
       </c>
       <c r="K444" s="2">
         <v>570.97460000000001</v>
       </c>
       <c r="L444" s="2" t="s">
-        <v>3537</v>
+        <v>3536</v>
       </c>
       <c r="M444" s="2">
         <v>0.233333333</v>
@@ -47318,7 +47318,7 @@
   <conditionalFormatting sqref="C10">
     <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1 D231:D266 D3:D228 D441:D443 D268 D270:D271 D273:D279 D281:D297 D299:D304 D306:D322 D324:D402 D404:D416 D418:D428 D431:D435 D437:D439">
+  <conditionalFormatting sqref="D1 D231:D266 D3:D193 D441:D443 D268 D270:D271 D273:D279 D281:D297 D299:D304 D306:D322 D324:D402 D404:D416 D418:D428 D431:D435 D437:D439 D195:D228">
     <cfRule type="duplicateValues" dxfId="6" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F444">
@@ -47361,54 +47361,54 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>3683</v>
+        <v>3682</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>3680</v>
+        <v>3679</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>3672</v>
+        <v>3671</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>3682</v>
+        <v>3681</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>3675</v>
+        <v>3674</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>3674</v>
+        <v>3673</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>3687</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>3688</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>3689</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>3690</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>3691</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>3691</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>3692</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>3693</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>3694</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>3692</v>
+        <v>3691</v>
       </c>
       <c r="E2" s="5">
         <v>386.35489999999999</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>3695</v>
+        <v>3694</v>
       </c>
       <c r="G2" s="8">
         <v>0.93333333333333302</v>
@@ -47425,22 +47425,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>3695</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>3696</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>3697</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>3694</v>
+        <v>3693</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>3696</v>
+        <v>3695</v>
       </c>
       <c r="E3" s="5">
         <v>161.1052</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>3698</v>
+        <v>3697</v>
       </c>
       <c r="G3" s="8">
         <v>3.3333333333333298E-2</v>
@@ -47457,22 +47457,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>3698</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>3699</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>3700</v>
-      </c>
       <c r="C4" s="5" t="s">
-        <v>3694</v>
+        <v>3693</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>3699</v>
+        <v>3698</v>
       </c>
       <c r="E4" s="5">
         <v>161.1052</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>3698</v>
+        <v>3697</v>
       </c>
       <c r="G4" s="8">
         <v>0.18333333333333299</v>
@@ -47489,22 +47489,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>3700</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>3701</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>3702</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>3703</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>3704</v>
       </c>
       <c r="E5" s="5">
         <v>352.22500000000002</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>3705</v>
+        <v>3704</v>
       </c>
       <c r="G5" s="8">
         <v>0.63333333333333297</v>
@@ -47521,22 +47521,22 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>3705</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>3706</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>3707</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>3708</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>3706</v>
+        <v>3705</v>
       </c>
       <c r="E6" s="5">
         <v>408.2876</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>3709</v>
+        <v>3708</v>
       </c>
       <c r="G6" s="8">
         <v>0.16666666666666699</v>
@@ -47553,22 +47553,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
+        <v>3709</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>3710</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>3711</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>3708</v>
+        <v>3707</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>3710</v>
+        <v>3709</v>
       </c>
       <c r="E7" s="5">
         <v>414.27460000000002</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>3712</v>
+        <v>3711</v>
       </c>
       <c r="G7" s="8">
         <v>6.6666666666666693E-2</v>
@@ -47585,22 +47585,22 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>3713</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
+        <v>3707</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>3714</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>3708</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>3715</v>
       </c>
       <c r="E8" s="5">
         <v>433.31920000000002</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>3716</v>
+        <v>3715</v>
       </c>
       <c r="G8" s="8">
         <v>1</v>
@@ -47617,22 +47617,22 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>3716</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>3717</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="9" t="s">
+        <v>3707</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>3718</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>3708</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>3719</v>
       </c>
       <c r="E9" s="5">
         <v>392.29259999999999</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>3720</v>
+        <v>3719</v>
       </c>
       <c r="G9" s="8">
         <v>1</v>
@@ -47649,22 +47649,22 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>3720</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>3721</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
+        <v>3707</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>3722</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>3708</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>3723</v>
       </c>
       <c r="E10" s="5">
         <v>376.29770000000002</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>3724</v>
+        <v>3723</v>
       </c>
       <c r="G10" s="8">
         <v>0.7</v>
@@ -47681,22 +47681,22 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>3724</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>3725</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>3726</v>
-      </c>
       <c r="C11" s="9" t="s">
-        <v>3708</v>
+        <v>3707</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>3725</v>
+        <v>3724</v>
       </c>
       <c r="E11" s="5">
         <v>392.29259999999999</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>3720</v>
+        <v>3719</v>
       </c>
       <c r="G11" s="8">
         <v>6.6666666666666693E-2</v>
@@ -47713,22 +47713,22 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
+        <v>3726</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>3727</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>3728</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>3729</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>3727</v>
+        <v>3726</v>
       </c>
       <c r="E12" s="5">
         <v>88.052400000000006</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>3730</v>
+        <v>3729</v>
       </c>
       <c r="G12" s="8">
         <v>1</v>
@@ -47745,16 +47745,16 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
+        <v>3730</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>3731</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>3732</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>3729</v>
+        <v>3728</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>3731</v>
+        <v>3730</v>
       </c>
       <c r="E13" s="5">
         <v>102.0681</v>
@@ -47777,22 +47777,22 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
+        <v>3732</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>3733</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="9" t="s">
         <v>3734</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>3735</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>3733</v>
+        <v>3732</v>
       </c>
       <c r="E14" s="5">
         <v>402.34980000000002</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>3736</v>
+        <v>3735</v>
       </c>
       <c r="G14" s="8">
         <v>1</v>
@@ -47809,22 +47809,22 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
+        <v>3736</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>3737</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>3738</v>
-      </c>
       <c r="C15" s="9" t="s">
-        <v>3735</v>
+        <v>3734</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>3737</v>
+        <v>3736</v>
       </c>
       <c r="E15" s="5">
         <v>332.23509999999999</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>3739</v>
+        <v>3738</v>
       </c>
       <c r="G15" s="8">
         <v>0.98333333333333295</v>
@@ -47841,22 +47841,22 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
+        <v>3739</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>3740</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>3741</v>
-      </c>
       <c r="C16" s="9" t="s">
-        <v>3735</v>
+        <v>3734</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>3740</v>
+        <v>3739</v>
       </c>
       <c r="E16" s="5">
         <v>384.33920000000001</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>3742</v>
+        <v>3741</v>
       </c>
       <c r="G16" s="8">
         <v>1</v>
@@ -47873,22 +47873,22 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>3742</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>3743</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>3744</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>3735</v>
+        <v>3734</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>3743</v>
+        <v>3742</v>
       </c>
       <c r="E17" s="5">
         <v>300.17250000000001</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>3745</v>
+        <v>3744</v>
       </c>
       <c r="G17" s="8">
         <v>1</v>
@@ -47905,22 +47905,22 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
+        <v>3745</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>3746</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>3747</v>
-      </c>
       <c r="C18" s="5" t="s">
-        <v>3735</v>
+        <v>3734</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>3746</v>
+        <v>3745</v>
       </c>
       <c r="E18" s="5">
         <v>272.17759999999998</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>3748</v>
+        <v>3747</v>
       </c>
       <c r="G18" s="8">
         <v>0.46666666666666701</v>
@@ -47937,22 +47937,22 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
+        <v>3748</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>3749</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>3750</v>
-      </c>
       <c r="C19" s="5" t="s">
-        <v>3735</v>
+        <v>3734</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>3749</v>
+        <v>3748</v>
       </c>
       <c r="E19" s="5">
         <v>288.17250000000001</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>3751</v>
+        <v>3750</v>
       </c>
       <c r="G19" s="8">
         <v>0.9</v>
@@ -47969,22 +47969,22 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
+        <v>3751</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>3752</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>3753</v>
-      </c>
       <c r="C20" s="5" t="s">
-        <v>3735</v>
+        <v>3734</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>3752</v>
+        <v>3751</v>
       </c>
       <c r="E20" s="5">
         <v>270.16199999999998</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>3754</v>
+        <v>3753</v>
       </c>
       <c r="G20" s="8">
         <v>1.6666666666666701E-2</v>
@@ -48001,22 +48001,22 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
+        <v>3754</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>3755</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>3756</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>3735</v>
+        <v>3734</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>3755</v>
+        <v>3754</v>
       </c>
       <c r="E21" s="5">
         <v>350.11878999999999</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>3757</v>
+        <v>3756</v>
       </c>
       <c r="G21" s="8">
         <v>0.71666666666666701</v>
@@ -48033,22 +48033,22 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
+        <v>3757</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>3758</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>3759</v>
-      </c>
       <c r="C22" s="5" t="s">
-        <v>3735</v>
+        <v>3734</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>3758</v>
+        <v>3757</v>
       </c>
       <c r="E22" s="5">
         <v>316.24023</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>3760</v>
+        <v>3759</v>
       </c>
       <c r="G22" s="8">
         <v>0.98333333333333295</v>
@@ -48065,22 +48065,22 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
+        <v>3760</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>3761</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>3762</v>
-      </c>
       <c r="C23" s="5" t="s">
-        <v>3735</v>
+        <v>3734</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>3761</v>
+        <v>3760</v>
       </c>
       <c r="E23" s="5">
         <v>314.22460000000001</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>3763</v>
+        <v>3762</v>
       </c>
       <c r="G23" s="8">
         <v>0.76666666666666705</v>
@@ -48097,22 +48097,22 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
+        <v>3763</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>3764</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>3765</v>
-      </c>
       <c r="C24" s="9" t="s">
-        <v>3735</v>
+        <v>3734</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>3764</v>
+        <v>3763</v>
       </c>
       <c r="E24" s="5">
         <v>288.20890000000003</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>3766</v>
+        <v>3765</v>
       </c>
       <c r="G24" s="8">
         <v>1</v>

</xml_diff>